<commit_message>
import excel with team names
</commit_message>
<xml_diff>
--- a/src/main/resources/excelimport/ConfederationsCup2017.xlsx
+++ b/src/main/resources/excelimport/ConfederationsCup2017.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Temp2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Temp1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="240">
   <si>
     <t>Country 1</t>
   </si>
@@ -722,6 +722,30 @@
   </si>
   <si>
     <t>Sotschi</t>
+  </si>
+  <si>
+    <t>Sieger Gruppe A</t>
+  </si>
+  <si>
+    <t>Zweiter Gruppe B</t>
+  </si>
+  <si>
+    <t>Sieger Gruppe B</t>
+  </si>
+  <si>
+    <t>Zweiter Gruppe A</t>
+  </si>
+  <si>
+    <t>Verlierer Halbfinale Kasan</t>
+  </si>
+  <si>
+    <t>Verlierer Halbfinale Sotschi</t>
+  </si>
+  <si>
+    <t>Sieger Halbfinale Kasan</t>
+  </si>
+  <si>
+    <t>Sieger Halbfinale Sotschi</t>
   </si>
 </sst>
 </file>
@@ -771,10 +795,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1092,12 +1117,12 @@
   <dimension ref="A1:E440"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
     <col min="3" max="3" width="24.140625" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
@@ -1326,60 +1351,116 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D14" s="2"/>
+      <c r="A14" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C14" t="s">
+        <v>225</v>
+      </c>
+      <c r="D14" s="2">
+        <v>42914.833333333336</v>
+      </c>
+      <c r="E14" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D15" s="2"/>
+      <c r="A15" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C15" t="s">
+        <v>225</v>
+      </c>
+      <c r="D15" s="2">
+        <v>42915.833333333336</v>
+      </c>
+      <c r="E15" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C16" t="s">
+        <v>227</v>
+      </c>
+      <c r="D16" s="2">
+        <v>42918.583333333336</v>
+      </c>
+      <c r="E16" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>238</v>
+      </c>
+      <c r="B17" t="s">
+        <v>239</v>
+      </c>
+      <c r="C17" t="s">
+        <v>226</v>
+      </c>
+      <c r="D17" s="2">
+        <v>42918.833333333336</v>
+      </c>
+      <c r="E17" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">
@@ -2612,18 +2693,24 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Countries!$A$1:$A$210</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:B440</xm:sqref>
+          <xm:sqref>A437:B440</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Groups!$A$1:$A$13</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C440</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
+          <x14:formula1>
+            <xm:f>Countries!$A$1:$A$210</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:B13 A16:B16 A18:B436</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2635,9 +2722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A210"/>
   <sheetViews>
-    <sheetView topLeftCell="A191" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>